<commit_message>
começando fazer a função de acuracia
</commit_message>
<xml_diff>
--- a/slither/0.8.0_smartbugs-curated/0.8.0_slither_smartbugs-curated_dasp.xlsx
+++ b/slither/0.8.0_smartbugs-curated/0.8.0_slither_smartbugs-curated_dasp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2217,1113 +2217,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="n">
-        <v>42</v>
-      </c>
-      <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" t="n">
-        <v>0</v>
-      </c>
-      <c r="K44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M44" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="n">
-        <v>43</v>
-      </c>
-      <c r="C45" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>0</v>
-      </c>
-      <c r="J45" t="n">
-        <v>1</v>
-      </c>
-      <c r="K45" t="n">
-        <v>0</v>
-      </c>
-      <c r="L45" t="n">
-        <v>0</v>
-      </c>
-      <c r="M45" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="n">
-        <v>44</v>
-      </c>
-      <c r="C46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" t="n">
-        <v>1</v>
-      </c>
-      <c r="K46" t="n">
-        <v>0</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="n">
-        <v>45</v>
-      </c>
-      <c r="C47" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" t="n">
-        <v>0</v>
-      </c>
-      <c r="J47" t="n">
-        <v>0</v>
-      </c>
-      <c r="K47" t="n">
-        <v>0</v>
-      </c>
-      <c r="L47" t="n">
-        <v>1</v>
-      </c>
-      <c r="M47" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="n">
-        <v>46</v>
-      </c>
-      <c r="C48" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0</v>
-      </c>
-      <c r="I48" t="n">
-        <v>0</v>
-      </c>
-      <c r="J48" t="n">
-        <v>0</v>
-      </c>
-      <c r="K48" t="n">
-        <v>0</v>
-      </c>
-      <c r="L48" t="n">
-        <v>2</v>
-      </c>
-      <c r="M48" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="n">
-        <v>47</v>
-      </c>
-      <c r="C49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" t="n">
-        <v>0</v>
-      </c>
-      <c r="J49" t="n">
-        <v>0</v>
-      </c>
-      <c r="K49" t="n">
-        <v>0</v>
-      </c>
-      <c r="L49" t="n">
-        <v>0</v>
-      </c>
-      <c r="M49" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="n">
-        <v>48</v>
-      </c>
-      <c r="C50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K50" t="n">
-        <v>0</v>
-      </c>
-      <c r="L50" t="n">
-        <v>1</v>
-      </c>
-      <c r="M50" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="n">
-        <v>49</v>
-      </c>
-      <c r="C51" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>1</v>
-      </c>
-      <c r="G51" t="n">
-        <v>0</v>
-      </c>
-      <c r="H51" t="n">
-        <v>0</v>
-      </c>
-      <c r="I51" t="n">
-        <v>0</v>
-      </c>
-      <c r="J51" t="n">
-        <v>0</v>
-      </c>
-      <c r="K51" t="n">
-        <v>0</v>
-      </c>
-      <c r="L51" t="n">
-        <v>0</v>
-      </c>
-      <c r="M51" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="n">
-        <v>50</v>
-      </c>
-      <c r="C52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" t="n">
-        <v>1</v>
-      </c>
-      <c r="F52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J52" t="n">
-        <v>0</v>
-      </c>
-      <c r="K52" t="n">
-        <v>0</v>
-      </c>
-      <c r="L52" t="n">
-        <v>0</v>
-      </c>
-      <c r="M52" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="n">
-        <v>51</v>
-      </c>
-      <c r="C53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
-        <v>1</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0</v>
-      </c>
-      <c r="H53" t="n">
-        <v>0</v>
-      </c>
-      <c r="I53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J53" t="n">
-        <v>0</v>
-      </c>
-      <c r="K53" t="n">
-        <v>0</v>
-      </c>
-      <c r="L53" t="n">
-        <v>0</v>
-      </c>
-      <c r="M53" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="n">
-        <v>52</v>
-      </c>
-      <c r="C54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0</v>
-      </c>
-      <c r="I54" t="n">
-        <v>0</v>
-      </c>
-      <c r="J54" t="n">
-        <v>0</v>
-      </c>
-      <c r="K54" t="n">
-        <v>0</v>
-      </c>
-      <c r="L54" t="n">
-        <v>0</v>
-      </c>
-      <c r="M54" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="n">
-        <v>53</v>
-      </c>
-      <c r="C55" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="n">
-        <v>1</v>
-      </c>
-      <c r="G55" t="n">
-        <v>1</v>
-      </c>
-      <c r="H55" t="n">
-        <v>0</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0</v>
-      </c>
-      <c r="J55" t="n">
-        <v>0</v>
-      </c>
-      <c r="K55" t="n">
-        <v>0</v>
-      </c>
-      <c r="L55" t="n">
-        <v>0</v>
-      </c>
-      <c r="M55" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="n">
-        <v>54</v>
-      </c>
-      <c r="C56" t="n">
-        <v>1</v>
-      </c>
-      <c r="D56" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K56" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="n">
-        <v>55</v>
-      </c>
-      <c r="C57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" t="n">
-        <v>0</v>
-      </c>
-      <c r="H57" t="n">
-        <v>0</v>
-      </c>
-      <c r="I57" t="n">
-        <v>0</v>
-      </c>
-      <c r="J57" t="n">
-        <v>0</v>
-      </c>
-      <c r="K57" t="n">
-        <v>0</v>
-      </c>
-      <c r="L57" t="n">
-        <v>13</v>
-      </c>
-      <c r="M57" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="n">
-        <v>56</v>
-      </c>
-      <c r="C58" t="n">
-        <v>1</v>
-      </c>
-      <c r="D58" t="n">
-        <v>0</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" t="n">
-        <v>9</v>
-      </c>
-      <c r="G58" t="n">
-        <v>1</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0</v>
-      </c>
-      <c r="I58" t="n">
-        <v>0</v>
-      </c>
-      <c r="J58" t="n">
-        <v>11</v>
-      </c>
-      <c r="K58" t="n">
-        <v>0</v>
-      </c>
-      <c r="L58" t="n">
-        <v>17</v>
-      </c>
-      <c r="M58" t="n">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="n">
-        <v>57</v>
-      </c>
-      <c r="C59" t="n">
-        <v>0</v>
-      </c>
-      <c r="D59" t="n">
-        <v>0</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="n">
-        <v>0</v>
-      </c>
-      <c r="H59" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" t="n">
-        <v>0</v>
-      </c>
-      <c r="J59" t="n">
-        <v>1</v>
-      </c>
-      <c r="K59" t="n">
-        <v>0</v>
-      </c>
-      <c r="L59" t="n">
-        <v>0</v>
-      </c>
-      <c r="M59" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="n">
-        <v>58</v>
-      </c>
-      <c r="C60" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" t="n">
-        <v>0</v>
-      </c>
-      <c r="E60" t="n">
-        <v>0</v>
-      </c>
-      <c r="F60" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" t="n">
-        <v>0</v>
-      </c>
-      <c r="I60" t="n">
-        <v>0</v>
-      </c>
-      <c r="J60" t="n">
-        <v>1</v>
-      </c>
-      <c r="K60" t="n">
-        <v>0</v>
-      </c>
-      <c r="L60" t="n">
-        <v>0</v>
-      </c>
-      <c r="M60" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="n">
-        <v>59</v>
-      </c>
-      <c r="C61" t="n">
-        <v>0</v>
-      </c>
-      <c r="D61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="n">
-        <v>60</v>
-      </c>
-      <c r="C62" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" t="n">
-        <v>0</v>
-      </c>
-      <c r="E62" t="n">
-        <v>0</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" t="n">
-        <v>0</v>
-      </c>
-      <c r="H62" t="n">
-        <v>0</v>
-      </c>
-      <c r="I62" t="n">
-        <v>0</v>
-      </c>
-      <c r="J62" t="n">
-        <v>0</v>
-      </c>
-      <c r="K62" t="n">
-        <v>0</v>
-      </c>
-      <c r="L62" t="n">
-        <v>0</v>
-      </c>
-      <c r="M62" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="n">
-        <v>61</v>
-      </c>
-      <c r="C63" t="n">
-        <v>0</v>
-      </c>
-      <c r="D63" t="n">
-        <v>0</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0</v>
-      </c>
-      <c r="F63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H63" t="n">
-        <v>0</v>
-      </c>
-      <c r="I63" t="n">
-        <v>0</v>
-      </c>
-      <c r="J63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K63" t="n">
-        <v>0</v>
-      </c>
-      <c r="L63" t="n">
-        <v>0</v>
-      </c>
-      <c r="M63" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="n">
-        <v>62</v>
-      </c>
-      <c r="C64" t="n">
-        <v>0</v>
-      </c>
-      <c r="D64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E64" t="n">
-        <v>0</v>
-      </c>
-      <c r="F64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" t="n">
-        <v>0</v>
-      </c>
-      <c r="H64" t="n">
-        <v>0</v>
-      </c>
-      <c r="I64" t="n">
-        <v>0</v>
-      </c>
-      <c r="J64" t="n">
-        <v>0</v>
-      </c>
-      <c r="K64" t="n">
-        <v>0</v>
-      </c>
-      <c r="L64" t="n">
-        <v>0</v>
-      </c>
-      <c r="M64" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B65" t="n">
-        <v>63</v>
-      </c>
-      <c r="C65" t="n">
-        <v>0</v>
-      </c>
-      <c r="D65" t="n">
-        <v>0</v>
-      </c>
-      <c r="E65" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" t="n">
-        <v>0</v>
-      </c>
-      <c r="H65" t="n">
-        <v>0</v>
-      </c>
-      <c r="I65" t="n">
-        <v>0</v>
-      </c>
-      <c r="J65" t="n">
-        <v>0</v>
-      </c>
-      <c r="K65" t="n">
-        <v>0</v>
-      </c>
-      <c r="L65" t="n">
-        <v>0</v>
-      </c>
-      <c r="M65" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B66" t="n">
-        <v>64</v>
-      </c>
-      <c r="C66" t="n">
-        <v>0</v>
-      </c>
-      <c r="D66" t="n">
-        <v>0</v>
-      </c>
-      <c r="E66" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" t="n">
-        <v>0</v>
-      </c>
-      <c r="H66" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" t="n">
-        <v>0</v>
-      </c>
-      <c r="K66" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B67" t="n">
-        <v>65</v>
-      </c>
-      <c r="C67" t="n">
-        <v>0</v>
-      </c>
-      <c r="D67" t="n">
-        <v>0</v>
-      </c>
-      <c r="E67" t="n">
-        <v>0</v>
-      </c>
-      <c r="F67" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" t="n">
-        <v>0</v>
-      </c>
-      <c r="H67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I67" t="n">
-        <v>0</v>
-      </c>
-      <c r="J67" t="n">
-        <v>0</v>
-      </c>
-      <c r="K67" t="n">
-        <v>0</v>
-      </c>
-      <c r="L67" t="n">
-        <v>0</v>
-      </c>
-      <c r="M67" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="n">
-        <v>66</v>
-      </c>
-      <c r="C68" t="n">
-        <v>0</v>
-      </c>
-      <c r="D68" t="n">
-        <v>0</v>
-      </c>
-      <c r="E68" t="n">
-        <v>0</v>
-      </c>
-      <c r="F68" t="n">
-        <v>0</v>
-      </c>
-      <c r="G68" t="n">
-        <v>0</v>
-      </c>
-      <c r="H68" t="n">
-        <v>0</v>
-      </c>
-      <c r="I68" t="n">
-        <v>0</v>
-      </c>
-      <c r="J68" t="n">
-        <v>0</v>
-      </c>
-      <c r="K68" t="n">
-        <v>0</v>
-      </c>
-      <c r="L68" t="n">
-        <v>0</v>
-      </c>
-      <c r="M68" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="n">
-        <v>67</v>
-      </c>
-      <c r="C69" t="n">
-        <v>1</v>
-      </c>
-      <c r="D69" t="n">
-        <v>0</v>
-      </c>
-      <c r="E69" t="n">
-        <v>0</v>
-      </c>
-      <c r="F69" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" t="n">
-        <v>0</v>
-      </c>
-      <c r="H69" t="n">
-        <v>0</v>
-      </c>
-      <c r="I69" t="n">
-        <v>0</v>
-      </c>
-      <c r="J69" t="n">
-        <v>0</v>
-      </c>
-      <c r="K69" t="n">
-        <v>0</v>
-      </c>
-      <c r="L69" t="n">
-        <v>0</v>
-      </c>
-      <c r="M69" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="n">
-        <v>68</v>
-      </c>
-      <c r="C70" t="n">
-        <v>1</v>
-      </c>
-      <c r="D70" t="n">
-        <v>0</v>
-      </c>
-      <c r="E70" t="n">
-        <v>0</v>
-      </c>
-      <c r="F70" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" t="n">
-        <v>0</v>
-      </c>
-      <c r="H70" t="n">
-        <v>0</v>
-      </c>
-      <c r="I70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J70" t="n">
-        <v>1</v>
-      </c>
-      <c r="K70" t="n">
-        <v>0</v>
-      </c>
-      <c r="L70" t="n">
-        <v>1</v>
-      </c>
-      <c r="M70" t="n">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
acertando problemas com a generalização
</commit_message>
<xml_diff>
--- a/slither/0.8.0_smartbugs-curated/0.8.0_slither_smartbugs-curated_dasp.xlsx
+++ b/slither/0.8.0_smartbugs-curated/0.8.0_slither_smartbugs-curated_dasp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2217,6 +2217,1113 @@
         <v>4</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>42</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>43</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>44</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>45</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>1</v>
+      </c>
+      <c r="M47" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>46</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" t="n">
+        <v>2</v>
+      </c>
+      <c r="M48" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>47</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>48</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" t="n">
+        <v>1</v>
+      </c>
+      <c r="M50" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>49</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>50</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>51</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>52</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>53</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>54</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>55</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" t="n">
+        <v>13</v>
+      </c>
+      <c r="M57" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>56</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>9</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>11</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" t="n">
+        <v>17</v>
+      </c>
+      <c r="M58" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>57</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>1</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>58</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="n">
+        <v>1</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>59</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>60</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>61</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0</v>
+      </c>
+      <c r="M63" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>62</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>63</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>64</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>65</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>66</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>67</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>68</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="n">
+        <v>1</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
+      <c r="L70" t="n">
+        <v>1</v>
+      </c>
+      <c r="M70" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>